<commit_message>
switch regression to be in different table
</commit_message>
<xml_diff>
--- a/output/evali_common_regression.xlsx
+++ b/output/evali_common_regression.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Table 5: The association between the EVALI case rate per million and marijuana policy while controling for both medical and recreational</t>
   </si>
@@ -35,58 +35,22 @@
     <t xml:space="preserve">(1)</t>
   </si>
   <si>
-    <t xml:space="preserve">OLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.06***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.86)</t>
+    <t xml:space="preserve">matrix.ncol...1..nrow...16.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-0.19 to 0.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.05***</t>
   </si>
   <si>
     <t xml:space="preserve">[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4.32 to 11.79)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2.8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.64]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-4.32 to 6.94)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.98*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2.01)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-9.03 to -0.934)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poisson (mfx)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-0.19 to 0.89)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3.05***</t>
   </si>
   <si>
     <t xml:space="preserve">(-3.59 to -2.51)</t>
@@ -511,7 +475,6 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -520,9 +483,6 @@
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
@@ -530,9 +490,6 @@
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -540,9 +497,6 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -551,9 +505,6 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -562,9 +513,6 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -573,9 +521,6 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -584,9 +529,6 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -595,9 +537,6 @@
         <v>3</v>
       </c>
       <c r="B9" s="7" t="n">
-        <v>1.31</v>
-      </c>
-      <c r="C9" s="7" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -606,10 +545,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -617,10 +553,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -628,10 +561,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -639,9 +569,6 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -650,10 +577,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -661,10 +585,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -672,10 +593,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -683,10 +601,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -694,9 +609,6 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -707,13 +619,10 @@
       <c r="B19" s="8" t="n">
         <v>51</v>
       </c>
-      <c r="C19" s="8" t="n">
-        <v>51</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>